<commit_message>
Update report form Cabo Verde and Timor Leste
</commit_message>
<xml_diff>
--- a/reports/Cabo Verde_3.2_imports_products_HS-AG6-2003-2022.xlsx
+++ b/reports/Cabo Verde_3.2_imports_products_HS-AG6-2003-2022.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrc/develop/cipf-comtrade/reports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495ACA18-48AB-544F-B7B6-AC6C21D8622B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4860" yWindow="500" windowWidth="29020" windowHeight="25660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -196,8 +202,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;MOP$&quot;_ ;_ * \(#,##0.00\)\ &quot;MOP$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;MOP$&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +218,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -246,27 +264,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -304,7 +342,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -338,6 +376,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -372,9 +411,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -547,14 +587,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="76.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,17 +620,17 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2003</v>
       </c>
@@ -602,17 +649,17 @@
       <c r="F2">
         <v>6</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="5">
         <v>34993412</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>0.04930970397715218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2" s="3">
+        <v>4.9309703977152182E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2003</v>
       </c>
@@ -631,17 +678,17 @@
       <c r="F3">
         <v>6</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>13098562</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>0.018457366053541</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3" s="3">
+        <v>1.8457366053541001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2003</v>
       </c>
@@ -660,17 +707,17 @@
       <c r="F4">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>10665667</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
-      <c r="I4">
-        <v>0.01502913984177595</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4" s="3">
+        <v>1.502913984177595E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -689,17 +736,17 @@
       <c r="F5">
         <v>6</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>8378430</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
-      <c r="I5">
-        <v>0.01180616234545208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" s="3">
+        <v>1.180616234545208E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2003</v>
       </c>
@@ -718,17 +765,17 @@
       <c r="F6">
         <v>6</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <v>7786766</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
-      <c r="I6">
-        <v>0.01097244036675684</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="3">
+        <v>1.097244036675684E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2004</v>
       </c>
@@ -747,17 +794,17 @@
       <c r="F7">
         <v>6</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>46799980</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>0.05451574626790138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="3">
+        <v>5.4515746267901379E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2004</v>
       </c>
@@ -776,17 +823,17 @@
       <c r="F8">
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
         <v>26298354</v>
       </c>
       <c r="H8">
         <v>2</v>
       </c>
-      <c r="I8">
-        <v>0.03063408133780077</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="3">
+        <v>3.0634081337800771E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2004</v>
       </c>
@@ -805,17 +852,17 @@
       <c r="F9">
         <v>6</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <v>16108574</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
-      <c r="I9">
-        <v>0.01876434419249139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" s="3">
+        <v>1.876434419249139E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2004</v>
       </c>
@@ -834,17 +881,17 @@
       <c r="F10">
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
         <v>9195550</v>
       </c>
       <c r="H10">
         <v>4</v>
       </c>
-      <c r="I10">
-        <v>0.01071159155610324</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="I10" s="3">
+        <v>1.0711591556103239E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2004</v>
       </c>
@@ -863,17 +910,17 @@
       <c r="F11">
         <v>6</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>8263356</v>
       </c>
       <c r="H11">
         <v>5</v>
       </c>
-      <c r="I11">
-        <v>0.009625709648109689</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" s="3">
+        <v>9.6257096481096888E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2005</v>
       </c>
@@ -892,17 +939,17 @@
       <c r="F12">
         <v>6</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>33672465</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12">
-        <v>0.03842325139857386</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" s="3">
+        <v>3.842325139857386E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2005</v>
       </c>
@@ -921,17 +968,17 @@
       <c r="F13">
         <v>6</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <v>18367317</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
-      <c r="I13">
-        <v>0.02095872810643056</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="I13" s="3">
+        <v>2.0958728106430562E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2005</v>
       </c>
@@ -950,17 +997,17 @@
       <c r="F14">
         <v>6</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
         <v>11372331</v>
       </c>
       <c r="H14">
         <v>3</v>
       </c>
-      <c r="I14">
-        <v>0.01297683234657144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="I14" s="3">
+        <v>1.2976832346571441E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2005</v>
       </c>
@@ -979,17 +1026,17 @@
       <c r="F15">
         <v>6</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="5">
         <v>9070769</v>
       </c>
       <c r="H15">
         <v>4</v>
       </c>
-      <c r="I15">
-        <v>0.01035054718047492</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="3">
+        <v>1.035054718047492E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2005</v>
       </c>
@@ -1008,17 +1055,17 @@
       <c r="F16">
         <v>6</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="5">
         <v>8359138</v>
       </c>
       <c r="H16">
         <v>5</v>
       </c>
-      <c r="I16">
-        <v>0.009538513466399679</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="I16" s="3">
+        <v>9.5385134663996795E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2006</v>
       </c>
@@ -1037,17 +1084,17 @@
       <c r="F17">
         <v>6</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="5">
         <v>43974884</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17">
-        <v>0.04085394500269501</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="3">
+        <v>4.0853945002695007E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -1066,17 +1113,17 @@
       <c r="F18">
         <v>6</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="5">
         <v>22124163</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
-      <c r="I18">
-        <v>0.02055399028301382</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="I18" s="3">
+        <v>2.0553990283013818E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -1095,17 +1142,17 @@
       <c r="F19">
         <v>6</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="5">
         <v>11031945</v>
       </c>
       <c r="H19">
         <v>3</v>
       </c>
-      <c r="I19">
-        <v>0.01024899745733852</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="3">
+        <v>1.024899745733852E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2006</v>
       </c>
@@ -1124,17 +1171,17 @@
       <c r="F20">
         <v>6</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="5">
         <v>10788930</v>
       </c>
       <c r="H20">
         <v>4</v>
       </c>
-      <c r="I20">
-        <v>0.01002322946111527</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="I20" s="3">
+        <v>1.0023229461115271E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2006</v>
       </c>
@@ -1153,17 +1200,17 @@
       <c r="F21">
         <v>6</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="5">
         <v>9232532</v>
       </c>
       <c r="H21">
         <v>5</v>
       </c>
-      <c r="I21">
-        <v>0.008577290495265929</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I21" s="3">
+        <v>8.5772904952659285E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2007</v>
       </c>
@@ -1182,17 +1229,17 @@
       <c r="F22">
         <v>6</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="5">
         <v>50498443</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22">
-        <v>0.03425982139332259</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="I22" s="3">
+        <v>3.4259821393322593E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2007</v>
       </c>
@@ -1211,17 +1258,17 @@
       <c r="F23">
         <v>6</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="5">
         <v>32056997</v>
       </c>
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23">
-        <v>0.02174853176416306</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="I23" s="3">
+        <v>2.1748531764163061E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2007</v>
       </c>
@@ -1240,17 +1287,17 @@
       <c r="F24">
         <v>6</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="5">
         <v>29204034</v>
       </c>
       <c r="H24">
         <v>3</v>
       </c>
-      <c r="I24">
-        <v>0.01981298688366531</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="I24" s="3">
+        <v>1.9812986883665309E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2007</v>
       </c>
@@ -1269,17 +1316,17 @@
       <c r="F25">
         <v>6</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="5">
         <v>18234970</v>
       </c>
       <c r="H25">
         <v>4</v>
       </c>
-      <c r="I25">
-        <v>0.0123712094512022</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="I25" s="3">
+        <v>1.23712094512022E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2007</v>
       </c>
@@ -1298,17 +1345,17 @@
       <c r="F26">
         <v>6</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="5">
         <v>18214320</v>
       </c>
       <c r="H26">
         <v>5</v>
       </c>
-      <c r="I26">
-        <v>0.01235719980516673</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="I26" s="3">
+        <v>1.2357199805166729E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2008</v>
       </c>
@@ -1327,17 +1374,17 @@
       <c r="F27">
         <v>6</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="5">
         <v>72707364</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27">
-        <v>0.0441100243702797</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="I27" s="3">
+        <v>4.41100243702797E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2008</v>
       </c>
@@ -1356,17 +1403,17 @@
       <c r="F28">
         <v>6</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="5">
         <v>35682349</v>
       </c>
       <c r="H28">
         <v>2</v>
       </c>
-      <c r="I28">
-        <v>0.02164772861217779</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="I28" s="3">
+        <v>2.1647728612177789E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2008</v>
       </c>
@@ -1385,17 +1432,17 @@
       <c r="F29">
         <v>6</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="5">
         <v>19181519</v>
       </c>
       <c r="H29">
         <v>3</v>
       </c>
-      <c r="I29">
-        <v>0.0116370230469225</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="I29" s="3">
+        <v>1.16370230469225E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2008</v>
       </c>
@@ -1414,17 +1461,17 @@
       <c r="F30">
         <v>6</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="5">
         <v>17639830</v>
       </c>
       <c r="H30">
         <v>4</v>
       </c>
-      <c r="I30">
-        <v>0.01070171284421191</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="I30" s="3">
+        <v>1.0701712844211911E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2008</v>
       </c>
@@ -1443,17 +1490,17 @@
       <c r="F31">
         <v>6</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="5">
         <v>15033793</v>
       </c>
       <c r="H31">
         <v>5</v>
       </c>
-      <c r="I31">
-        <v>0.009120685156564614</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="I31" s="3">
+        <v>9.1206851565646136E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2009</v>
       </c>
@@ -1472,17 +1519,17 @@
       <c r="F32">
         <v>6</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="5">
         <v>63950428</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
-      <c r="I32">
-        <v>0.04765119090780529</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="I32" s="3">
+        <v>4.7651190907805292E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2009</v>
       </c>
@@ -1501,17 +1548,17 @@
       <c r="F33">
         <v>6</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="5">
         <v>29137009</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
-      <c r="I33">
-        <v>0.02171077226162491</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="I33" s="3">
+        <v>2.1710772261624909E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2009</v>
       </c>
@@ -1530,17 +1577,17 @@
       <c r="F34">
         <v>6</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="5">
         <v>27152937</v>
       </c>
       <c r="H34">
         <v>3</v>
       </c>
-      <c r="I34">
-        <v>0.02023238663382534</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="I34" s="3">
+        <v>2.0232386633825341E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2009</v>
       </c>
@@ -1559,17 +1606,17 @@
       <c r="F35">
         <v>6</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="5">
         <v>10853612</v>
       </c>
       <c r="H35">
         <v>4</v>
       </c>
-      <c r="I35">
-        <v>0.00808731940701392</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="I35" s="3">
+        <v>8.0873194070139199E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2009</v>
       </c>
@@ -1588,17 +1635,17 @@
       <c r="F36">
         <v>6</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="5">
         <v>10477601</v>
       </c>
       <c r="H36">
         <v>5</v>
       </c>
-      <c r="I36">
-        <v>0.007807143456597533</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="I36" s="3">
+        <v>7.8071434565975331E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2010</v>
       </c>
@@ -1617,17 +1664,17 @@
       <c r="F37">
         <v>6</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="5">
         <v>69762739</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37">
-        <v>0.04773262560360782</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="I37" s="3">
+        <v>4.7732625603607817E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2010</v>
       </c>
@@ -1646,17 +1693,17 @@
       <c r="F38">
         <v>6</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="5">
         <v>26093163</v>
       </c>
       <c r="H38">
         <v>2</v>
       </c>
-      <c r="I38">
-        <v>0.01785330103356338</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="I38" s="3">
+        <v>1.785330103356338E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2010</v>
       </c>
@@ -1675,17 +1722,17 @@
       <c r="F39">
         <v>6</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="5">
         <v>24764094</v>
       </c>
       <c r="H39">
         <v>3</v>
       </c>
-      <c r="I39">
-        <v>0.0169439337425463</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="I39" s="3">
+        <v>1.69439337425463E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2010</v>
       </c>
@@ -1704,17 +1751,17 @@
       <c r="F40">
         <v>6</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="5">
         <v>15585536</v>
       </c>
       <c r="H40">
         <v>4</v>
       </c>
-      <c r="I40">
-        <v>0.01066383810875819</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="I40" s="3">
+        <v>1.066383810875819E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2010</v>
       </c>
@@ -1733,17 +1780,17 @@
       <c r="F41">
         <v>6</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="5">
         <v>12234751</v>
       </c>
       <c r="H41">
         <v>5</v>
       </c>
-      <c r="I41">
-        <v>0.008371184922030747</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="I41" s="3">
+        <v>8.3711849220307472E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2011</v>
       </c>
@@ -1762,17 +1809,17 @@
       <c r="F42">
         <v>6</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="5">
         <v>160049800</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
-      <c r="I42">
-        <v>0.08454312196152505</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="I42" s="3">
+        <v>8.4543121961525053E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -1791,17 +1838,17 @@
       <c r="F43">
         <v>6</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="5">
         <v>28503793</v>
       </c>
       <c r="H43">
         <v>2</v>
       </c>
-      <c r="I43">
-        <v>0.01505656144503188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="I43" s="3">
+        <v>1.5056561445031881E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -1820,17 +1867,17 @@
       <c r="F44">
         <v>6</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="5">
         <v>24715866</v>
       </c>
       <c r="H44">
         <v>3</v>
       </c>
-      <c r="I44">
-        <v>0.01305566438460223</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="I44" s="3">
+        <v>1.305566438460223E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2011</v>
       </c>
@@ -1849,17 +1896,17 @@
       <c r="F45">
         <v>6</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="5">
         <v>17091797</v>
       </c>
       <c r="H45">
         <v>4</v>
       </c>
-      <c r="I45">
-        <v>0.009028401649440536</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="I45" s="3">
+        <v>9.0284016494405362E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -1878,17 +1925,17 @@
       <c r="F46">
         <v>6</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="5">
         <v>14888836</v>
       </c>
       <c r="H46">
         <v>5</v>
       </c>
-      <c r="I46">
-        <v>0.007864731338702984</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="I46" s="3">
+        <v>7.8647313387029839E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2012</v>
       </c>
@@ -1907,17 +1954,17 @@
       <c r="F47">
         <v>6</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="5">
         <v>89183480</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
-      <c r="I47">
-        <v>0.05908093478889756</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="I47" s="3">
+        <v>5.908093478889756E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2012</v>
       </c>
@@ -1936,17 +1983,17 @@
       <c r="F48">
         <v>6</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="5">
         <v>57615688</v>
       </c>
       <c r="H48">
         <v>2</v>
       </c>
-      <c r="I48">
-        <v>0.03816837721005581</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="I48" s="3">
+        <v>3.8168377210055809E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2012</v>
       </c>
@@ -1965,17 +2012,17 @@
       <c r="F49">
         <v>6</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="5">
         <v>22817998</v>
       </c>
       <c r="H49">
         <v>3</v>
       </c>
-      <c r="I49">
-        <v>0.0151161252269052</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="I49" s="3">
+        <v>1.5116125226905201E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2012</v>
       </c>
@@ -1994,17 +2041,17 @@
       <c r="F50">
         <v>6</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="5">
         <v>22302940</v>
       </c>
       <c r="H50">
         <v>4</v>
       </c>
-      <c r="I50">
-        <v>0.01477491732483073</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="I50" s="3">
+        <v>1.477491732483073E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2012</v>
       </c>
@@ -2023,17 +2070,17 @@
       <c r="F51">
         <v>6</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="5">
         <v>12362905</v>
       </c>
       <c r="H51">
         <v>5</v>
       </c>
-      <c r="I51">
-        <v>0.008189991959344216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="I51" s="3">
+        <v>8.1899919593442158E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2013</v>
       </c>
@@ -2052,17 +2099,17 @@
       <c r="F52">
         <v>6</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="5">
         <v>134431171.692</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
-      <c r="I52">
-        <v>0.09255460197684853</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="I52" s="3">
+        <v>9.2554601976848533E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2013</v>
       </c>
@@ -2081,17 +2128,17 @@
       <c r="F53">
         <v>6</v>
       </c>
-      <c r="G53">
-        <v>27120806.006</v>
+      <c r="G53" s="5">
+        <v>27120806.006000001</v>
       </c>
       <c r="H53">
         <v>2</v>
       </c>
-      <c r="I53">
-        <v>0.01867242079037858</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="I53" s="3">
+        <v>1.8672420790378581E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2013</v>
       </c>
@@ -2110,17 +2157,17 @@
       <c r="F54">
         <v>6</v>
       </c>
-      <c r="G54">
-        <v>21999442.475</v>
+      <c r="G54" s="5">
+        <v>21999442.475000001</v>
       </c>
       <c r="H54">
         <v>3</v>
       </c>
-      <c r="I54">
-        <v>0.01514640999076684</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="I54" s="3">
+        <v>1.514640999076684E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2013</v>
       </c>
@@ -2139,17 +2186,17 @@
       <c r="F55">
         <v>6</v>
       </c>
-      <c r="G55">
-        <v>11946917.028</v>
+      <c r="G55" s="5">
+        <v>11946917.028000001</v>
       </c>
       <c r="H55">
         <v>4</v>
       </c>
-      <c r="I55">
-        <v>0.008225340421121816</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="I55" s="3">
+        <v>8.2253404211218156E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2013</v>
       </c>
@@ -2168,17 +2215,17 @@
       <c r="F56">
         <v>6</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="5">
         <v>11832380.088</v>
       </c>
       <c r="H56">
         <v>5</v>
       </c>
-      <c r="I56">
-        <v>0.008146482811239232</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="I56" s="3">
+        <v>8.1464828112392321E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2014</v>
       </c>
@@ -2197,17 +2244,17 @@
       <c r="F57">
         <v>6</v>
       </c>
-      <c r="G57">
-        <v>99802370.25300001</v>
+      <c r="G57" s="5">
+        <v>99802370.253000006</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
-      <c r="I57">
-        <v>0.06501389148470244</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="I57" s="3">
+        <v>6.5013891484702435E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2014</v>
       </c>
@@ -2226,17 +2273,17 @@
       <c r="F58">
         <v>6</v>
       </c>
-      <c r="G58">
-        <v>23751331.896</v>
+      <c r="G58" s="5">
+        <v>23751331.896000002</v>
       </c>
       <c r="H58">
         <v>2</v>
       </c>
-      <c r="I58">
-        <v>0.01547224289953453</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="I58" s="3">
+        <v>1.5472242899534531E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2014</v>
       </c>
@@ -2255,17 +2302,17 @@
       <c r="F59">
         <v>6</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="5">
         <v>20707327.088</v>
       </c>
       <c r="H59">
         <v>3</v>
       </c>
-      <c r="I59">
-        <v>0.0134892980279394</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="I59" s="3">
+        <v>1.3489298027939399E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2014</v>
       </c>
@@ -2284,17 +2331,17 @@
       <c r="F60">
         <v>6</v>
       </c>
-      <c r="G60">
-        <v>20342993.117</v>
+      <c r="G60" s="5">
+        <v>20342993.116999999</v>
       </c>
       <c r="H60">
         <v>4</v>
       </c>
-      <c r="I60">
-        <v>0.01325196128739167</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="I60" s="3">
+        <v>1.3251961287391671E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2014</v>
       </c>
@@ -2313,17 +2360,17 @@
       <c r="F61">
         <v>6</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="5">
         <v>16235654.547</v>
       </c>
       <c r="H61">
         <v>5</v>
       </c>
-      <c r="I61">
-        <v>0.01057633280878962</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="I61" s="3">
+        <v>1.0576332808789619E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2015</v>
       </c>
@@ -2342,17 +2389,17 @@
       <c r="F62">
         <v>6</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="5">
         <v>64738531.353</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
-      <c r="I62">
-        <v>0.05364212834179172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="I62" s="3">
+        <v>5.3642128341791717E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2015</v>
       </c>
@@ -2371,17 +2418,17 @@
       <c r="F63">
         <v>6</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="5">
         <v>21441812.616</v>
       </c>
       <c r="H63">
         <v>2</v>
       </c>
-      <c r="I63">
-        <v>0.0177666134864337</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="I63" s="3">
+        <v>1.7766613486433699E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2015</v>
       </c>
@@ -2400,17 +2447,17 @@
       <c r="F64">
         <v>6</v>
       </c>
-      <c r="G64">
-        <v>18316843.795</v>
+      <c r="G64" s="5">
+        <v>18316843.795000002</v>
       </c>
       <c r="H64">
         <v>3</v>
       </c>
-      <c r="I64">
-        <v>0.01517727487993763</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="I64" s="3">
+        <v>1.5177274879937631E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2015</v>
       </c>
@@ -2429,17 +2476,17 @@
       <c r="F65">
         <v>6</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="5">
         <v>10587190.804</v>
       </c>
       <c r="H65">
         <v>4</v>
       </c>
-      <c r="I65">
-        <v>0.008772510528397821</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="I65" s="3">
+        <v>8.772510528397821E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2015</v>
       </c>
@@ -2458,17 +2505,17 @@
       <c r="F66">
         <v>6</v>
       </c>
-      <c r="G66">
-        <v>9892268.473999999</v>
+      <c r="G66" s="5">
+        <v>9892268.4739999995</v>
       </c>
       <c r="H66">
         <v>5</v>
       </c>
-      <c r="I66">
-        <v>0.008196700233750019</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="I66" s="3">
+        <v>8.1967002337500188E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2016</v>
       </c>
@@ -2487,17 +2534,17 @@
       <c r="F67">
         <v>6</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="5">
         <v>49451740</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
-      <c r="I67">
-        <v>0.03678568034450681</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="I67" s="3">
+        <v>3.6785680344506813E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2016</v>
       </c>
@@ -2516,17 +2563,17 @@
       <c r="F68">
         <v>6</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="5">
         <v>21157608</v>
       </c>
       <c r="H68">
         <v>2</v>
       </c>
-      <c r="I68">
-        <v>0.01573851607127231</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="I68" s="3">
+        <v>1.5738516071272309E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2016</v>
       </c>
@@ -2545,17 +2592,17 @@
       <c r="F69">
         <v>6</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="5">
         <v>16119035</v>
       </c>
       <c r="H69">
         <v>3</v>
       </c>
-      <c r="I69">
-        <v>0.01199047129528541</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="I69" s="3">
+        <v>1.199047129528541E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2016</v>
       </c>
@@ -2574,17 +2621,17 @@
       <c r="F70">
         <v>6</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="5">
         <v>10928508</v>
       </c>
       <c r="H70">
         <v>4</v>
       </c>
-      <c r="I70">
-        <v>0.008129392452730387</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="I70" s="3">
+        <v>8.1293924527303871E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2016</v>
       </c>
@@ -2603,17 +2650,17 @@
       <c r="F71">
         <v>6</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="5">
         <v>9847750</v>
       </c>
       <c r="H71">
         <v>5</v>
       </c>
-      <c r="I71">
-        <v>0.007325448682141758</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="I71" s="3">
+        <v>7.325448682141758E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2017</v>
       </c>
@@ -2632,17 +2679,17 @@
       <c r="F72">
         <v>6</v>
       </c>
-      <c r="G72">
-        <v>64693216.314</v>
+      <c r="G72" s="5">
+        <v>64693216.314000003</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
-      <c r="I72">
-        <v>0.04075938523579396</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="I72" s="3">
+        <v>4.0759385235793963E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2017</v>
       </c>
@@ -2661,17 +2708,17 @@
       <c r="F73">
         <v>6</v>
       </c>
-      <c r="G73">
-        <v>27550465.876</v>
+      <c r="G73" s="5">
+        <v>27550465.875999998</v>
       </c>
       <c r="H73">
         <v>2</v>
       </c>
-      <c r="I73">
-        <v>0.01735792585446812</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="I73" s="3">
+        <v>1.7357925854468121E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2017</v>
       </c>
@@ -2690,17 +2737,17 @@
       <c r="F74">
         <v>6</v>
       </c>
-      <c r="G74">
-        <v>22447695.448</v>
+      <c r="G74" s="5">
+        <v>22447695.447999999</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
-      <c r="I74">
-        <v>0.01414297075569589</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="I74" s="3">
+        <v>1.4142970755695891E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2017</v>
       </c>
@@ -2719,17 +2766,17 @@
       <c r="F75">
         <v>6</v>
       </c>
-      <c r="G75">
-        <v>19442562.889</v>
+      <c r="G75" s="5">
+        <v>19442562.888999999</v>
       </c>
       <c r="H75">
         <v>4</v>
       </c>
-      <c r="I75">
-        <v>0.01224961372947549</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="I75" s="3">
+        <v>1.224961372947549E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2017</v>
       </c>
@@ -2748,17 +2795,17 @@
       <c r="F76">
         <v>6</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="5">
         <v>11664139.705</v>
       </c>
       <c r="H76">
         <v>5</v>
       </c>
-      <c r="I76">
-        <v>0.007348887422332882</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="I76" s="3">
+        <v>7.3488874223328823E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2018</v>
       </c>
@@ -2777,17 +2824,17 @@
       <c r="F77">
         <v>6</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="5">
         <v>1732522.35</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
-      <c r="I77">
-        <v>0.001063413461523375</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="I77" s="3">
+        <v>1.0634134615233751E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2018</v>
       </c>
@@ -2806,17 +2853,17 @@
       <c r="F78">
         <v>6</v>
       </c>
-      <c r="G78">
+      <c r="G78" s="5">
         <v>20136684.77</v>
       </c>
       <c r="H78">
         <v>2</v>
       </c>
-      <c r="I78">
-        <v>0.01235979533243581</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="I78" s="3">
+        <v>1.235979533243581E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2018</v>
       </c>
@@ -2835,17 +2882,17 @@
       <c r="F79">
         <v>6</v>
       </c>
-      <c r="G79">
+      <c r="G79" s="5">
         <v>444.91</v>
       </c>
       <c r="H79">
         <v>3</v>
       </c>
-      <c r="I79">
-        <v>2.730835092351707E-07</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="I79" s="3">
+        <v>2.7308350923517068E-7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2018</v>
       </c>
@@ -2864,17 +2911,17 @@
       <c r="F80">
         <v>6</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="5">
         <v>49976.65</v>
       </c>
       <c r="H80">
         <v>4</v>
       </c>
-      <c r="I80">
-        <v>3.067541516670314E-05</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="I80" s="3">
+        <v>3.067541516670314E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2018</v>
       </c>
@@ -2893,17 +2940,17 @@
       <c r="F81">
         <v>6</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="5">
         <v>10582177.32</v>
       </c>
       <c r="H81">
         <v>5</v>
       </c>
-      <c r="I81">
-        <v>0.006495286952180067</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="I81" s="3">
+        <v>6.4952869521800669E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2019</v>
       </c>
@@ -2922,17 +2969,17 @@
       <c r="F82">
         <v>6</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="5">
         <v>1821.91</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
-      <c r="I82">
-        <v>1.153537111223886E-06</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="I82" s="3">
+        <v>1.1535371112238859E-6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2019</v>
       </c>
@@ -2951,17 +2998,17 @@
       <c r="F83">
         <v>6</v>
       </c>
-      <c r="G83">
+      <c r="G83" s="5">
         <v>2.99</v>
       </c>
       <c r="H83">
         <v>2</v>
       </c>
-      <c r="I83">
-        <v>1.89310995743995E-09</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="I83" s="3">
+        <v>1.8931099574399502E-9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2019</v>
       </c>
@@ -2980,17 +3027,17 @@
       <c r="F84">
         <v>6</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="5">
         <v>9.65</v>
       </c>
       <c r="H84">
         <v>3</v>
       </c>
-      <c r="I84">
-        <v>6.109869929530273E-09</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="I84" s="3">
+        <v>6.1098699295302731E-9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2019</v>
       </c>
@@ -3009,17 +3056,17 @@
       <c r="F85">
         <v>6</v>
       </c>
-      <c r="G85">
+      <c r="G85" s="5">
         <v>85280.03</v>
       </c>
       <c r="H85">
         <v>4</v>
       </c>
-      <c r="I85">
-        <v>5.399480734574503E-05</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="I85" s="3">
+        <v>5.3994807345745032E-5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2019</v>
       </c>
@@ -3038,17 +3085,17 @@
       <c r="F86">
         <v>6</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="5">
         <v>2622.08</v>
       </c>
       <c r="H86">
         <v>5</v>
       </c>
-      <c r="I86">
-        <v>1.660162460603393E-06</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="I86" s="3">
+        <v>1.660162460603393E-6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2020</v>
       </c>
@@ -3067,17 +3114,17 @@
       <c r="F87">
         <v>6</v>
       </c>
-      <c r="G87">
-        <v>140810617.696</v>
+      <c r="G87" s="5">
+        <v>140810617.69600001</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
-      <c r="I87">
-        <v>0.06222853226764937</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="I87" s="3">
+        <v>6.2228532267649371E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2020</v>
       </c>
@@ -3096,17 +3143,17 @@
       <c r="F88">
         <v>6</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="5">
         <v>11364.133</v>
       </c>
       <c r="H88">
         <v>2</v>
       </c>
-      <c r="I88">
-        <v>5.02215904351116E-06</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="I88" s="3">
+        <v>5.0221590435111604E-6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2020</v>
       </c>
@@ -3125,17 +3172,17 @@
       <c r="F89">
         <v>6</v>
       </c>
-      <c r="G89">
-        <v>29765566.086</v>
+      <c r="G89" s="5">
+        <v>29765566.085999999</v>
       </c>
       <c r="H89">
         <v>3</v>
       </c>
-      <c r="I89">
-        <v>0.0131543169112887</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="I89" s="3">
+        <v>1.31543169112887E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2020</v>
       </c>
@@ -3154,17 +3201,17 @@
       <c r="F90">
         <v>6</v>
       </c>
-      <c r="G90">
-        <v>21716.383</v>
+      <c r="G90" s="5">
+        <v>21716.383000000002</v>
       </c>
       <c r="H90">
         <v>4</v>
       </c>
-      <c r="I90">
-        <v>9.597135943041324E-06</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="I90" s="3">
+        <v>9.5971359430413238E-6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2020</v>
       </c>
@@ -3183,17 +3230,17 @@
       <c r="F91">
         <v>6</v>
       </c>
-      <c r="G91">
-        <v>14837961.735</v>
+      <c r="G91" s="5">
+        <v>14837961.734999999</v>
       </c>
       <c r="H91">
         <v>5</v>
       </c>
-      <c r="I91">
-        <v>0.006557350544445651</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="I91" s="3">
+        <v>6.5573505444456509E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2021</v>
       </c>
@@ -3212,17 +3259,17 @@
       <c r="F92">
         <v>6</v>
       </c>
-      <c r="G92">
-        <v>3338779.998</v>
+      <c r="G92" s="5">
+        <v>3338779.9980000001</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
-      <c r="I92">
-        <v>0.002185524253168035</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="I92" s="3">
+        <v>2.185524253168035E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2021</v>
       </c>
@@ -3241,17 +3288,17 @@
       <c r="F93">
         <v>6</v>
       </c>
-      <c r="G93">
-        <v>26648322.075</v>
+      <c r="G93" s="5">
+        <v>26648322.074999999</v>
       </c>
       <c r="H93">
         <v>2</v>
       </c>
-      <c r="I93">
-        <v>0.01744366332493694</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="I93" s="3">
+        <v>1.744366332493694E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2021</v>
       </c>
@@ -3270,17 +3317,17 @@
       <c r="F94">
         <v>6</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="5">
         <v>111.745</v>
       </c>
       <c r="H94">
         <v>3</v>
       </c>
-      <c r="I94">
-        <v>7.314690030986044E-08</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="I94" s="3">
+        <v>7.3146900309860436E-8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2021</v>
       </c>
@@ -3299,17 +3346,17 @@
       <c r="F95">
         <v>6</v>
       </c>
-      <c r="G95">
+      <c r="G95" s="5">
         <v>13767133.874</v>
       </c>
       <c r="H95">
         <v>4</v>
       </c>
-      <c r="I95">
-        <v>0.009011796223848768</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="I95" s="3">
+        <v>9.0117962238487684E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2021</v>
       </c>
@@ -3328,17 +3375,17 @@
       <c r="F96">
         <v>6</v>
       </c>
-      <c r="G96">
-        <v>284584.106</v>
+      <c r="G96" s="5">
+        <v>284584.10600000003</v>
       </c>
       <c r="H96">
         <v>5</v>
       </c>
-      <c r="I96">
-        <v>0.0001862852497324512</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="I96" s="3">
+        <v>1.862852497324512E-4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2022</v>
       </c>
@@ -3357,17 +3404,17 @@
       <c r="F97">
         <v>6</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="5">
         <v>125706.514</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
-      <c r="I97">
-        <v>7.553339952123864E-05</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="I97" s="3">
+        <v>7.5533399521238639E-5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2022</v>
       </c>
@@ -3386,17 +3433,17 @@
       <c r="F98">
         <v>6</v>
       </c>
-      <c r="G98">
-        <v>14206.691</v>
+      <c r="G98" s="5">
+        <v>14206.691000000001</v>
       </c>
       <c r="H98">
         <v>2</v>
       </c>
-      <c r="I98">
-        <v>8.536388712344575E-06</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="I98" s="3">
+        <v>8.5363887123445754E-6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2022</v>
       </c>
@@ -3415,17 +3462,17 @@
       <c r="F99">
         <v>6</v>
       </c>
-      <c r="G99">
-        <v>376.301</v>
+      <c r="G99" s="5">
+        <v>376.30099999999999</v>
       </c>
       <c r="H99">
         <v>3</v>
       </c>
-      <c r="I99">
-        <v>2.261083604087663E-07</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="I99" s="3">
+        <v>2.2610836040876631E-7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2022</v>
       </c>
@@ -3444,17 +3491,17 @@
       <c r="F100">
         <v>6</v>
       </c>
-      <c r="G100">
-        <v>112897.081</v>
+      <c r="G100" s="5">
+        <v>112897.08100000001</v>
       </c>
       <c r="H100">
         <v>4</v>
       </c>
-      <c r="I100">
-        <v>6.78365826289212E-05</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="I100" s="3">
+        <v>6.7836582628921202E-5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2022</v>
       </c>
@@ -3473,17 +3520,50 @@
       <c r="F101">
         <v>6</v>
       </c>
-      <c r="G101">
+      <c r="G101" s="5">
         <v>398669.43</v>
       </c>
       <c r="H101">
         <v>5</v>
       </c>
-      <c r="I101">
-        <v>0.0002395489014443156</v>
+      <c r="I101" s="3">
+        <v>2.3954890144431559E-4</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{73A9928D-9F05-6249-8A05-3DBD341F6DDE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{73A9928D-9F05-6249-8A05-3DBD341F6DDE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>